<commit_message>
gpt few shot learning
</commit_message>
<xml_diff>
--- a/ComparissonTable_Thesis.xlsx
+++ b/ComparissonTable_Thesis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strat\Desktop\EKPA\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BG\Desktop\EKPA\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F9BCF-5BB4-45C3-BE8D-641B27EFEA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33C0477-3132-48CD-8B25-E30F22EEB13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21600" xr2:uid="{3BEB7030-4BE0-4DE3-B2A0-E298BEBA13B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3BEB7030-4BE0-4DE3-B2A0-E298BEBA13B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Model</t>
   </si>
@@ -74,7 +74,10 @@
     <t>WAT</t>
   </si>
   <si>
-    <t>GPT-3.5</t>
+    <t>GPT-(one)</t>
+  </si>
+  <si>
+    <t>GPT-(few)</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,6 +218,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258AD91F-87AC-4732-AC34-8BB3F74463ED}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="151" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,19 +640,43 @@
       </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="6"/>
+      <c r="B5" s="12">
+        <v>1044</v>
+      </c>
+      <c r="C5" s="12">
+        <v>301</v>
+      </c>
+      <c r="D5" s="12">
+        <v>88</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:G1"/>

</xml_diff>